<commit_message>
Updates on Sprint documents
</commit_message>
<xml_diff>
--- a/Scrum/Templates/2/Agile-product-backlog-template.xlsx
+++ b/Scrum/Templates/2/Agile-product-backlog-template.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisma\Documents\Visual Studio 2015\Projects\WindowsFormsApplication3\Scrum\Templates\2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12000" yWindow="0" windowWidth="29060" windowHeight="19640" tabRatio="500"/>
+    <workbookView xWindow="12000" yWindow="0" windowWidth="29055" windowHeight="19635" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +20,7 @@
     <definedName name="Status">Sheet2!$C$6:$C$8</definedName>
     <definedName name="YesNo">Sheet2!$A$6:$A$7</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="37">
   <si>
     <t>Task Name</t>
   </si>
@@ -51,48 +56,9 @@
     <t>Sprint 1</t>
   </si>
   <si>
-    <t>Task 1</t>
-  </si>
-  <si>
-    <t>Task 2</t>
-  </si>
-  <si>
-    <t>Task 3</t>
-  </si>
-  <si>
-    <t>Sprint 2</t>
-  </si>
-  <si>
-    <t>Task 4</t>
-  </si>
-  <si>
-    <t>Task 5</t>
-  </si>
-  <si>
-    <t>Task 6</t>
-  </si>
-  <si>
-    <t>Sprint 3</t>
-  </si>
-  <si>
-    <t>Task 7</t>
-  </si>
-  <si>
-    <t>Task 8</t>
-  </si>
-  <si>
-    <t>Task 9</t>
-  </si>
-  <si>
     <t>Sprint 4</t>
   </si>
   <si>
-    <t>Task 10</t>
-  </si>
-  <si>
-    <t>Task 11</t>
-  </si>
-  <si>
     <t>Task 12</t>
   </si>
   <si>
@@ -139,13 +105,49 @@
   </si>
   <si>
     <t>Create a Product Backlog in Smartsheet</t>
+  </si>
+  <si>
+    <t>Extract MLB Stats</t>
+  </si>
+  <si>
+    <t>Extract MLB Schedule</t>
+  </si>
+  <si>
+    <t>Extract MLB Series</t>
+  </si>
+  <si>
+    <t>Align MLB Series per day</t>
+  </si>
+  <si>
+    <t>Create class/DB model with data</t>
+  </si>
+  <si>
+    <t>Create MLB Game Class</t>
+  </si>
+  <si>
+    <t>Extract data from team</t>
+  </si>
+  <si>
+    <t>Fill data periodically</t>
+  </si>
+  <si>
+    <t>Creting of sheets depending of quantities and dates</t>
+  </si>
+  <si>
+    <t>Order schedule</t>
+  </si>
+  <si>
+    <t>Create MLB Serie class</t>
+  </si>
+  <si>
+    <t>http://www.covers.com/pageLoader/pageLoader.aspx?page=/data/mlb/matchups/g4_summary_12.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -194,8 +196,15 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -226,6 +235,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -251,11 +265,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -270,16 +285,28 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -688,22 +715,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:L34"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.1640625" customWidth="1"/>
+    <col min="1" max="1" width="33.125" customWidth="1"/>
     <col min="2" max="2" width="11.5" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
-    <col min="6" max="6" width="13.83203125" customWidth="1"/>
+    <col min="3" max="3" width="13.875" customWidth="1"/>
+    <col min="4" max="4" width="15.375" customWidth="1"/>
+    <col min="5" max="5" width="16.625" customWidth="1"/>
+    <col min="6" max="6" width="13.875" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -734,7 +761,7 @@
       <c r="AB1" s="5"/>
       <c r="AC1" s="5"/>
     </row>
-    <row r="2" spans="1:29">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -764,9 +791,9 @@
       <c r="AB2" s="5"/>
       <c r="AC2" s="5"/>
     </row>
-    <row r="3" spans="1:29" ht="23">
+    <row r="3" spans="1:29" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -797,7 +824,7 @@
       <c r="AB3" s="5"/>
       <c r="AC3" s="5"/>
     </row>
-    <row r="4" spans="1:29">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -828,7 +855,7 @@
       <c r="AB4" s="5"/>
       <c r="AC4" s="5"/>
     </row>
-    <row r="5" spans="1:29">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -859,7 +886,7 @@
       <c r="AB5" s="5"/>
       <c r="AC5" s="5"/>
     </row>
-    <row r="6" spans="1:29" ht="36" customHeight="1">
+    <row r="6" spans="1:29" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -904,28 +931,28 @@
       <c r="AB6" s="5"/>
       <c r="AC6" s="5"/>
     </row>
-    <row r="7" spans="1:29" ht="22" customHeight="1">
+    <row r="7" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="F7" s="3">
         <f>SUM(F8:F10)</f>
         <v>24</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
@@ -950,27 +977,27 @@
       <c r="AB7" s="5"/>
       <c r="AC7" s="5"/>
     </row>
-    <row r="8" spans="1:29" ht="22" customHeight="1">
-      <c r="A8" s="2" t="s">
-        <v>8</v>
+    <row r="8" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="F8" s="2">
         <v>8</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
@@ -995,27 +1022,27 @@
       <c r="AB8" s="5"/>
       <c r="AC8" s="5"/>
     </row>
-    <row r="9" spans="1:29" ht="22" customHeight="1">
-      <c r="A9" s="2" t="s">
-        <v>9</v>
+    <row r="9" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="F9" s="2">
         <v>16</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
@@ -1040,27 +1067,27 @@
       <c r="AB9" s="5"/>
       <c r="AC9" s="5"/>
     </row>
-    <row r="10" spans="1:29" ht="22" customHeight="1">
-      <c r="A10" s="2" t="s">
-        <v>10</v>
+    <row r="10" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="F10" s="2">
         <v>0</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
@@ -1085,29 +1112,16 @@
       <c r="AB10" s="5"/>
       <c r="AC10" s="5"/>
     </row>
-    <row r="11" spans="1:29" ht="22" customHeight="1">
-      <c r="A11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>27</v>
-      </c>
+    <row r="11" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
       <c r="D11" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" s="3">
-        <f>SUM(F12:F14)</f>
-        <v>96</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>27</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
@@ -1131,27 +1145,27 @@
       <c r="AB11" s="5"/>
       <c r="AC11" s="5"/>
     </row>
-    <row r="12" spans="1:29" ht="22" customHeight="1">
-      <c r="A12" s="2" t="s">
-        <v>12</v>
+    <row r="12" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>28</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="F12" s="2">
         <v>32</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
@@ -1176,27 +1190,27 @@
       <c r="AB12" s="5"/>
       <c r="AC12" s="5"/>
     </row>
-    <row r="13" spans="1:29" ht="22" customHeight="1">
-      <c r="A13" s="2" t="s">
-        <v>13</v>
+    <row r="13" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="F13" s="2">
         <v>48</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
@@ -1221,27 +1235,27 @@
       <c r="AB13" s="5"/>
       <c r="AC13" s="5"/>
     </row>
-    <row r="14" spans="1:29" ht="22" customHeight="1">
-      <c r="A14" s="2" t="s">
-        <v>14</v>
+    <row r="14" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="F14" s="2">
         <v>16</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
@@ -1266,29 +1280,14 @@
       <c r="AB14" s="5"/>
       <c r="AC14" s="5"/>
     </row>
-    <row r="15" spans="1:29" ht="22" customHeight="1">
-      <c r="A15" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F15" s="3">
-        <f>SUM(F16:F18)</f>
-        <v>32</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>28</v>
-      </c>
+    <row r="15" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -1312,27 +1311,27 @@
       <c r="AB15" s="5"/>
       <c r="AC15" s="5"/>
     </row>
-    <row r="16" spans="1:29" ht="22" customHeight="1">
-      <c r="A16" s="2" t="s">
-        <v>16</v>
+    <row r="16" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="F16" s="2">
         <v>8</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
@@ -1357,27 +1356,27 @@
       <c r="AB16" s="5"/>
       <c r="AC16" s="5"/>
     </row>
-    <row r="17" spans="1:29" ht="22" customHeight="1">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="E17" s="2" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="F17" s="2">
         <v>8</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
@@ -1402,27 +1401,27 @@
       <c r="AB17" s="5"/>
       <c r="AC17" s="5"/>
     </row>
-    <row r="18" spans="1:29" ht="22" customHeight="1">
+    <row r="18" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="E18" s="2" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="F18" s="2">
         <v>16</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
@@ -1447,28 +1446,28 @@
       <c r="AB18" s="5"/>
       <c r="AC18" s="5"/>
     </row>
-    <row r="19" spans="1:29" ht="22" customHeight="1">
+    <row r="19" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="F19" s="3">
         <f>SUM(F20:F22)</f>
         <v>64</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
@@ -1493,27 +1492,27 @@
       <c r="AB19" s="5"/>
       <c r="AC19" s="5"/>
     </row>
-    <row r="20" spans="1:29" ht="22" customHeight="1">
-      <c r="A20" s="2" t="s">
+    <row r="20" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="F20" s="2">
         <v>32</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
@@ -1538,27 +1537,27 @@
       <c r="AB20" s="5"/>
       <c r="AC20" s="5"/>
     </row>
-    <row r="21" spans="1:29" ht="22" customHeight="1">
+    <row r="21" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="F21" s="2">
         <v>32</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
@@ -1583,27 +1582,27 @@
       <c r="AB21" s="5"/>
       <c r="AC21" s="5"/>
     </row>
-    <row r="22" spans="1:29" ht="22" customHeight="1">
+    <row r="22" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="F22" s="2">
         <v>0</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
@@ -1628,28 +1627,28 @@
       <c r="AB22" s="5"/>
       <c r="AC22" s="5"/>
     </row>
-    <row r="23" spans="1:29" ht="22" customHeight="1">
+    <row r="23" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="F23" s="3">
         <f>SUM(F24:F26)</f>
         <v>64</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
@@ -1674,27 +1673,27 @@
       <c r="AB23" s="5"/>
       <c r="AC23" s="5"/>
     </row>
-    <row r="24" spans="1:29" ht="22" customHeight="1">
+    <row r="24" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="F24" s="2">
         <v>48</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
@@ -1719,27 +1718,27 @@
       <c r="AB24" s="5"/>
       <c r="AC24" s="5"/>
     </row>
-    <row r="25" spans="1:29" ht="22" customHeight="1">
+    <row r="25" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="F25" s="2">
         <v>8</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
@@ -1764,27 +1763,27 @@
       <c r="AB25" s="5"/>
       <c r="AC25" s="5"/>
     </row>
-    <row r="26" spans="1:29" ht="22" customHeight="1">
+    <row r="26" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="F26" s="2">
         <v>8</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
@@ -1809,7 +1808,7 @@
       <c r="AB26" s="5"/>
       <c r="AC26" s="5"/>
     </row>
-    <row r="27" spans="1:29">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -1840,7 +1839,7 @@
       <c r="AB27" s="5"/>
       <c r="AC27" s="5"/>
     </row>
-    <row r="28" spans="1:29">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -1871,21 +1870,21 @@
       <c r="AB28" s="5"/>
       <c r="AC28" s="5"/>
     </row>
-    <row r="29" spans="1:29">
-      <c r="A29" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
       <c r="M29" s="7"/>
       <c r="N29" s="5"/>
       <c r="O29" s="5"/>
@@ -1904,19 +1903,19 @@
       <c r="AB29" s="5"/>
       <c r="AC29" s="5"/>
     </row>
-    <row r="30" spans="1:29">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A30" s="9"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9"/>
       <c r="M30" s="7"/>
       <c r="N30" s="5"/>
       <c r="O30" s="5"/>
@@ -1935,19 +1934,19 @@
       <c r="AB30" s="5"/>
       <c r="AC30" s="5"/>
     </row>
-    <row r="31" spans="1:29">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
+    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A31" s="9"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="9"/>
       <c r="M31" s="7"/>
       <c r="N31" s="5"/>
       <c r="O31" s="5"/>
@@ -1966,19 +1965,19 @@
       <c r="AB31" s="5"/>
       <c r="AC31" s="5"/>
     </row>
-    <row r="32" spans="1:29">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
-      <c r="K32" s="8"/>
-      <c r="L32" s="8"/>
+    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A32" s="9"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="9"/>
       <c r="M32" s="7"/>
       <c r="N32" s="5"/>
       <c r="O32" s="5"/>
@@ -1997,19 +1996,19 @@
       <c r="AB32" s="5"/>
       <c r="AC32" s="5"/>
     </row>
-    <row r="33" spans="1:29">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
+    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A33" s="9"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9"/>
+      <c r="L33" s="9"/>
       <c r="M33" s="7"/>
       <c r="N33" s="5"/>
       <c r="O33" s="5"/>
@@ -2028,19 +2027,19 @@
       <c r="AB33" s="5"/>
       <c r="AC33" s="5"/>
     </row>
-    <row r="34" spans="1:29">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
-      <c r="K34" s="8"/>
-      <c r="L34" s="8"/>
+    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A34" s="9"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="9"/>
+      <c r="L34" s="9"/>
       <c r="M34" s="7"/>
       <c r="N34" s="5"/>
       <c r="O34" s="5"/>
@@ -2059,7 +2058,7 @@
       <c r="AB34" s="5"/>
       <c r="AC34" s="5"/>
     </row>
-    <row r="35" spans="1:29">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
@@ -2090,7 +2089,7 @@
       <c r="AB35" s="5"/>
       <c r="AC35" s="5"/>
     </row>
-    <row r="36" spans="1:29">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -2121,7 +2120,7 @@
       <c r="AB36" s="5"/>
       <c r="AC36" s="5"/>
     </row>
-    <row r="37" spans="1:29">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -2152,7 +2151,7 @@
       <c r="AB37" s="5"/>
       <c r="AC37" s="5"/>
     </row>
-    <row r="38" spans="1:29">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
@@ -2183,7 +2182,7 @@
       <c r="AB38" s="5"/>
       <c r="AC38" s="5"/>
     </row>
-    <row r="39" spans="1:29">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
@@ -2214,7 +2213,7 @@
       <c r="AB39" s="5"/>
       <c r="AC39" s="5"/>
     </row>
-    <row r="40" spans="1:29">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -2245,7 +2244,7 @@
       <c r="AB40" s="5"/>
       <c r="AC40" s="5"/>
     </row>
-    <row r="41" spans="1:29">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
@@ -2276,7 +2275,7 @@
       <c r="AB41" s="5"/>
       <c r="AC41" s="5"/>
     </row>
-    <row r="42" spans="1:29">
+    <row r="42" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
@@ -2307,7 +2306,7 @@
       <c r="AB42" s="5"/>
       <c r="AC42" s="5"/>
     </row>
-    <row r="43" spans="1:29">
+    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
@@ -2338,7 +2337,7 @@
       <c r="AB43" s="5"/>
       <c r="AC43" s="5"/>
     </row>
-    <row r="44" spans="1:29">
+    <row r="44" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
@@ -2369,7 +2368,7 @@
       <c r="AB44" s="5"/>
       <c r="AC44" s="5"/>
     </row>
-    <row r="45" spans="1:29">
+    <row r="45" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
@@ -2400,7 +2399,7 @@
       <c r="AB45" s="5"/>
       <c r="AC45" s="5"/>
     </row>
-    <row r="46" spans="1:29">
+    <row r="46" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
@@ -2431,7 +2430,7 @@
       <c r="AB46" s="5"/>
       <c r="AC46" s="5"/>
     </row>
-    <row r="47" spans="1:29">
+    <row r="47" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
@@ -2462,7 +2461,7 @@
       <c r="AB47" s="5"/>
       <c r="AC47" s="5"/>
     </row>
-    <row r="48" spans="1:29">
+    <row r="48" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
@@ -2493,7 +2492,7 @@
       <c r="AB48" s="5"/>
       <c r="AC48" s="5"/>
     </row>
-    <row r="49" spans="1:29">
+    <row r="49" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
@@ -2524,7 +2523,7 @@
       <c r="AB49" s="5"/>
       <c r="AC49" s="5"/>
     </row>
-    <row r="50" spans="1:29">
+    <row r="50" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A50" s="5"/>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
@@ -2555,7 +2554,7 @@
       <c r="AB50" s="5"/>
       <c r="AC50" s="5"/>
     </row>
-    <row r="51" spans="1:29">
+    <row r="51" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A51" s="5"/>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
@@ -2586,7 +2585,7 @@
       <c r="AB51" s="5"/>
       <c r="AC51" s="5"/>
     </row>
-    <row r="52" spans="1:29">
+    <row r="52" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A52" s="5"/>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
@@ -2617,7 +2616,7 @@
       <c r="AB52" s="5"/>
       <c r="AC52" s="5"/>
     </row>
-    <row r="53" spans="1:29">
+    <row r="53" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A53" s="5"/>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
@@ -2648,7 +2647,7 @@
       <c r="AB53" s="5"/>
       <c r="AC53" s="5"/>
     </row>
-    <row r="54" spans="1:29">
+    <row r="54" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A54" s="5"/>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
@@ -2679,7 +2678,7 @@
       <c r="AB54" s="5"/>
       <c r="AC54" s="5"/>
     </row>
-    <row r="55" spans="1:29">
+    <row r="55" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A55" s="5"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
@@ -2710,7 +2709,7 @@
       <c r="AB55" s="5"/>
       <c r="AC55" s="5"/>
     </row>
-    <row r="56" spans="1:29">
+    <row r="56" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A56" s="5"/>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
@@ -2741,7 +2740,7 @@
       <c r="AB56" s="5"/>
       <c r="AC56" s="5"/>
     </row>
-    <row r="57" spans="1:29">
+    <row r="57" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A57" s="5"/>
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
@@ -2772,7 +2771,7 @@
       <c r="AB57" s="5"/>
       <c r="AC57" s="5"/>
     </row>
-    <row r="58" spans="1:29">
+    <row r="58" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A58" s="5"/>
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
@@ -2803,7 +2802,7 @@
       <c r="AB58" s="5"/>
       <c r="AC58" s="5"/>
     </row>
-    <row r="59" spans="1:29">
+    <row r="59" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A59" s="5"/>
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
@@ -2834,7 +2833,7 @@
       <c r="AB59" s="5"/>
       <c r="AC59" s="5"/>
     </row>
-    <row r="60" spans="1:29">
+    <row r="60" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A60" s="5"/>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
@@ -2865,7 +2864,7 @@
       <c r="AB60" s="5"/>
       <c r="AC60" s="5"/>
     </row>
-    <row r="61" spans="1:29">
+    <row r="61" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A61" s="5"/>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
@@ -2896,7 +2895,7 @@
       <c r="AB61" s="5"/>
       <c r="AC61" s="5"/>
     </row>
-    <row r="62" spans="1:29">
+    <row r="62" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A62" s="5"/>
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
@@ -2927,7 +2926,7 @@
       <c r="AB62" s="5"/>
       <c r="AC62" s="5"/>
     </row>
-    <row r="63" spans="1:29">
+    <row r="63" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A63" s="5"/>
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
@@ -2958,7 +2957,7 @@
       <c r="AB63" s="5"/>
       <c r="AC63" s="5"/>
     </row>
-    <row r="64" spans="1:29">
+    <row r="64" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A64" s="5"/>
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
@@ -2989,7 +2988,7 @@
       <c r="AB64" s="5"/>
       <c r="AC64" s="5"/>
     </row>
-    <row r="65" spans="1:29">
+    <row r="65" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A65" s="5"/>
       <c r="B65" s="5"/>
       <c r="C65" s="5"/>
@@ -3020,7 +3019,7 @@
       <c r="AB65" s="5"/>
       <c r="AC65" s="5"/>
     </row>
-    <row r="66" spans="1:29">
+    <row r="66" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A66" s="5"/>
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
@@ -3051,7 +3050,7 @@
       <c r="AB66" s="5"/>
       <c r="AC66" s="5"/>
     </row>
-    <row r="67" spans="1:29">
+    <row r="67" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A67" s="5"/>
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
@@ -3082,7 +3081,7 @@
       <c r="AB67" s="5"/>
       <c r="AC67" s="5"/>
     </row>
-    <row r="68" spans="1:29">
+    <row r="68" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A68" s="5"/>
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
@@ -3113,7 +3112,7 @@
       <c r="AB68" s="5"/>
       <c r="AC68" s="5"/>
     </row>
-    <row r="69" spans="1:29">
+    <row r="69" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A69" s="5"/>
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
@@ -3144,7 +3143,7 @@
       <c r="AB69" s="5"/>
       <c r="AC69" s="5"/>
     </row>
-    <row r="70" spans="1:29">
+    <row r="70" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A70" s="5"/>
       <c r="B70" s="5"/>
       <c r="C70" s="5"/>
@@ -3175,7 +3174,7 @@
       <c r="AB70" s="5"/>
       <c r="AC70" s="5"/>
     </row>
-    <row r="71" spans="1:29">
+    <row r="71" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A71" s="5"/>
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
@@ -3206,7 +3205,7 @@
       <c r="AB71" s="5"/>
       <c r="AC71" s="5"/>
     </row>
-    <row r="72" spans="1:29">
+    <row r="72" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A72" s="5"/>
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
@@ -3344,41 +3343,41 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>